<commit_message>
Clarifying and making more consistent the DISPLAY strings. Plus some field name changes for consistency
</commit_message>
<xml_diff>
--- a/src/other/build_assets/toml_config_data.xlsx
+++ b/src/other/build_assets/toml_config_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrush/src.GitHub/trueblocks-core/src/other/build_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D303D51-5599-9F42-B861-0612C190FA54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA2D823-BE8A-E747-891E-9D2F7EC44334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="357">
   <si>
     <t>acctExport</t>
   </si>
@@ -990,18 +990,9 @@
     <t>----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
   </si>
   <si>
-    <t>hash, timestamp, from, to, ether, blockNumber, transactionIndex, etherGasPrice, gasUsed, isError, encoding</t>
-  </si>
-  <si>
     <t>blockNumber, transactionIndex, logIndex, address, topic0, topic1, topic2, topic3, data, type, compressedLog</t>
   </si>
   <si>
-    <t>blockNumber, transactionPosition, traceAddress, action::callType, error, action::from, action::to, action:value, action::ether, action::gas, result::gasUsed, action::input, compressedTrace, result::output</t>
-  </si>
-  <si>
-    <t>address, blockNum, tx_id, priorBalance, balance</t>
-  </si>
-  <si>
     <t>blockNumber, timestamp, date, name</t>
   </si>
   <si>
@@ -1029,9 +1020,6 @@
     <t>STR_DISPLAY_WHERE</t>
   </si>
   <si>
-    <t>STR_DISPLAY_ACCOUNTNAME2</t>
-  </si>
-  <si>
     <t>STR_DISPLAY_ACCOUNTNAME</t>
   </si>
   <si>
@@ -1047,9 +1035,6 @@
     <t>CBalanceRecord</t>
   </si>
   <si>
-    <t>date, timestamp, blockNumber, transactionIndex, hash, compressedTx</t>
-  </si>
-  <si>
     <t>CTransaction</t>
   </si>
   <si>
@@ -1062,18 +1047,12 @@
     <t>CAccountName</t>
   </si>
   <si>
-    <t>address, name, symbol</t>
-  </si>
-  <si>
     <t>group, address, name, symbol, source, description, logo, is_contract, is_private, is_shared</t>
   </si>
   <si>
     <t>CEthState</t>
   </si>
   <si>
-    <t>address, blockNumber, balance, nonce, code, storage, deployed, acctType</t>
-  </si>
-  <si>
     <t>blockNumber, transactionIndex, hash, gasUsed, status, isError</t>
   </si>
   <si>
@@ -1089,9 +1068,6 @@
     <t>CBlock</t>
   </si>
   <si>
-    <t>STR_DISPLAY_TRANSACTION2</t>
-  </si>
-  <si>
     <t>STR_DISPLAY_TRANSACTION</t>
   </si>
   <si>
@@ -1105,6 +1081,18 @@
   </si>
   <si>
     <t>name, type, anonymous, constant, payable, signature, encoding, inputs, outputs</t>
+  </si>
+  <si>
+    <t>blockNumber, transactionIndex, traceAddress, action::callType, error, action::from, action::to, action:value, action::ether, action::gas, result::gasUsed, action::input, compressedTrace, result::output</t>
+  </si>
+  <si>
+    <t>blockNumber, transactionIndex, address, priorBalance, balance</t>
+  </si>
+  <si>
+    <t>blockNumber, transactionIndex, date, timestamp, from, to, ether, etherGasPrice, gasUsed, hash, isError, encoding, compressedTx</t>
+  </si>
+  <si>
+    <t>blockNumber, address, balance, nonce, code, storage, deployed, acctType</t>
   </si>
 </sst>
 </file>
@@ -3291,7 +3279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="147" zoomScaleNormal="147" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6709,7 +6699,7 @@
   <dimension ref="B2:J76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6745,7 +6735,7 @@
         <v>226</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>70</v>
@@ -6766,14 +6756,14 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" t="s">
-        <v>342</v>
-      </c>
-      <c r="I3" t="s">
-        <v>322</v>
+        <v>337</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>355</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>226</v>
@@ -6793,14 +6783,14 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>226</v>
@@ -6820,14 +6810,14 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="I5" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>226</v>
@@ -6847,14 +6837,14 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G6" s="53"/>
       <c r="H6" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I6" t="s">
-        <v>325</v>
+        <v>354</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>226</v>
@@ -6903,11 +6893,11 @@
         <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G8" s="53"/>
       <c r="H8" s="8" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>226</v>
@@ -6956,14 +6946,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>226</v>
@@ -7012,14 +7002,14 @@
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="12" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>226</v>
@@ -7068,14 +7058,14 @@
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="I14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>226</v>
@@ -7124,14 +7114,14 @@
         <v>12</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="I16" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>226</v>
@@ -7180,14 +7170,14 @@
         <v>12</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="I18" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>226</v>
@@ -7236,14 +7226,14 @@
         <v>12</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="I20" t="s">
-        <v>346</v>
+        <v>340</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>226</v>
@@ -7251,99 +7241,105 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="18">
-        <v>286</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>347</v>
+        <v>287</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>321</v>
       </c>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="18">
-        <v>287</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>321</v>
+        <v>288</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>352</v>
       </c>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="18">
-        <v>288</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>360</v>
+        <v>290</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>321</v>
       </c>
       <c r="J23" s="3"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="18">
-        <v>290</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>321</v>
+        <v>295</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>338</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>226</v>
@@ -7351,26 +7347,28 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="18">
-        <v>295</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>343</v>
+        <v>300</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>321</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>226</v>
@@ -7378,28 +7376,24 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="18">
-        <v>300</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H26" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>321</v>
+        <v>310</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="12" t="s">
+        <v>323</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>226</v>
@@ -7407,24 +7401,28 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="18">
-        <v>310</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="12" t="s">
-        <v>326</v>
+        <v>315</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>321</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>226</v>
@@ -7432,28 +7430,24 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="18">
-        <v>315</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="I28" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="12" t="s">
+        <v>324</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>226</v>
@@ -7461,61 +7455,41 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" s="18">
-        <v>320</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="12" t="s">
-        <v>327</v>
+        <v>999</v>
+      </c>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="26" t="s">
+        <v>226</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="18">
-        <v>999</v>
-      </c>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="26" t="s">
-        <v>226</v>
-      </c>
+      <c r="B30" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="21">
-        <v>1000</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
       <c r="J31" s="4"/>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C76" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="B3:I29">
-    <sortCondition ref="B3:B29"/>
+  <sortState ref="B3:I30">
+    <sortCondition ref="B3:B30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working on cleaning up makeClass a bit and adding default display strings
</commit_message>
<xml_diff>
--- a/src/other/build_assets/toml_config_data.xlsx
+++ b/src/other/build_assets/toml_config_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrush/src.GitHub/trueblocks-core/src/other/build_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA2D823-BE8A-E747-891E-9D2F7EC44334}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FEE3AC-6622-8B4F-B7A7-37E5FB5E0083}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,21 +999,12 @@
     <t>blockNumber, path, cached</t>
   </si>
   <si>
-    <t>STR_DISPLAY_LOG</t>
-  </si>
-  <si>
     <t>STR_DISPLAY_RECEIPT</t>
   </si>
   <si>
     <t>STR_DISPLAY_TRACE</t>
   </si>
   <si>
-    <t>STR_DISPLAY_STATE</t>
-  </si>
-  <si>
-    <t>STR_DISPLAY_ETHQUOTE</t>
-  </si>
-  <si>
     <t>STR_DISPLAY_WHEN</t>
   </si>
   <si>
@@ -1093,6 +1084,15 @@
   </si>
   <si>
     <t>blockNumber, address, balance, nonce, code, storage, deployed, acctType</t>
+  </si>
+  <si>
+    <t>STR_DISPLAY_PRICEQUOTE</t>
+  </si>
+  <si>
+    <t>STR_DISPLAY_LOGENTRY</t>
+  </si>
+  <si>
+    <t>STR_DISPLAY_ETHSTATE</t>
   </si>
 </sst>
 </file>
@@ -6699,7 +6699,7 @@
   <dimension ref="B2:J76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6735,7 +6735,7 @@
         <v>226</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>70</v>
@@ -6756,14 +6756,14 @@
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>226</v>
@@ -6783,11 +6783,11 @@
         <v>13</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>325</v>
+        <v>355</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I4" t="s">
         <v>322</v>
@@ -6810,14 +6810,14 @@
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>226</v>
@@ -6837,14 +6837,14 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G6" s="53"/>
       <c r="H6" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I6" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>226</v>
@@ -6893,11 +6893,11 @@
         <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G8" s="53"/>
       <c r="H8" s="8" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>226</v>
@@ -6946,14 +6946,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>226</v>
@@ -7002,14 +7002,14 @@
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>226</v>
@@ -7058,11 +7058,11 @@
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>325</v>
+        <v>355</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I14" t="s">
         <v>322</v>
@@ -7114,14 +7114,14 @@
         <v>12</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="I16" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>226</v>
@@ -7170,14 +7170,14 @@
         <v>12</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>328</v>
+        <v>356</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>226</v>
@@ -7226,14 +7226,14 @@
         <v>12</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>226</v>
@@ -7271,7 +7271,7 @@
         <v>288</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>10</v>
@@ -7280,14 +7280,14 @@
         <v>12</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J22" s="3"/>
     </row>
@@ -7332,14 +7332,14 @@
         <v>12</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>329</v>
+        <v>354</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>226</v>
@@ -7388,7 +7388,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -7442,7 +7442,7 @@
         <v>12</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>

</xml_diff>

<commit_message>
Cleaning up issue #1201
</commit_message>
<xml_diff>
--- a/src/other/build_assets/toml_config_data.xlsx
+++ b/src/other/build_assets/toml_config_data.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrush/src.GitHub/trueblocks-core/src/other/build_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF66113-1154-0B42-877B-4D325B58AF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89434F9A-66E0-7741-B182-B7BED3B4D0BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="460" windowWidth="43120" windowHeight="28340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="460" windowWidth="43120" windowHeight="28340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Screen and JSON data" sheetId="1" r:id="rId1"/>
     <sheet name="Config Items" sheetId="2" r:id="rId2"/>
     <sheet name="Display Strings" sheetId="3" r:id="rId3"/>
+    <sheet name="Env Vars" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="366">
   <si>
     <t>acctExport</t>
   </si>
@@ -1093,6 +1094,33 @@
   </si>
   <si>
     <t>blockNumber, transactionIndex, traceAddress, action::callType, error, action::from, action::to, action::value, action::ether, action::gas, result::gasUsed, action::input, compressedTrace, result::output</t>
+  </si>
+  <si>
+    <t>env var</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>TEST_MODE</t>
+  </si>
+  <si>
+    <t>DOCKER_MODE</t>
+  </si>
+  <si>
+    <t>API_MODE</t>
+  </si>
+  <si>
+    <t>EDITOR</t>
+  </si>
+  <si>
+    <t>IPFS_PATH</t>
+  </si>
+  <si>
+    <t>NO_COLOR</t>
+  </si>
+  <si>
+    <t>NO_SOURCE</t>
   </si>
 </sst>
 </file>
@@ -6698,7 +6726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98772D29-303E-8043-9AC6-25CBD08E65CB}">
   <dimension ref="B2:J76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7493,4 +7521,145 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6AD0C4-4A68-084B-9562-3908CF754C73}">
+  <dimension ref="B2:E57"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="175.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="18">
+        <v>140</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="18">
+        <v>145</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="18">
+        <v>150</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="18">
+        <v>160</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="18">
+        <v>205</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="18">
+        <v>215</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="18">
+        <v>220</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="18">
+        <v>999</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="21">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57" s="4"/>
+    </row>
+  </sheetData>
+  <sortState ref="B3:D11">
+    <sortCondition ref="B3:B11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>